<commit_message>
ajouter analyse et conception pour les OA
</commit_message>
<xml_diff>
--- a/doc/grille-pointage.xlsx
+++ b/doc/grille-pointage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvanross/sources/log430/LOG430-STM/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755BA5CF-F831-184E-89F7-BE3849DF4FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC7E152-B332-FA40-8116-D4ABFB55A227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1160" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementation" sheetId="5" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t xml:space="preserve"> OA1 - Faciliter le recrutement des nouveaux chargés de laboratoire.</t>
   </si>
   <si>
-    <t xml:space="preserve"> OA2 - Validez si le transport par autobus est toujours plus rapide, peu importe l'heure de la journée</t>
-  </si>
-  <si>
     <t>CU03 - Comparer l’impact écologique de divers trajets en autobus et en auto</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t>Nom étudiants</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OA2 - Promouvoir l'utilisation des données ouvertes</t>
   </si>
 </sst>
 </file>
@@ -1153,6 +1153,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1160,12 +1166,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1392,8 +1392,8 @@
   </sheetPr>
   <dimension ref="B1:AG825"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="3" spans="2:31" ht="23.25" customHeight="1">
       <c r="B3" s="96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="97">
         <v>1</v>
@@ -1716,14 +1716,14 @@
       <c r="C9" s="28"/>
       <c r="D9" s="29"/>
       <c r="E9" s="51"/>
-      <c r="F9" s="107" t="s">
+      <c r="F9" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="109"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="111"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1746,18 +1746,18 @@
       <c r="C10" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="110"/>
-      <c r="E10" s="111"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="108"/>
       <c r="F10" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="110"/>
-      <c r="H10" s="111"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="108"/>
       <c r="I10" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="110"/>
-      <c r="K10" s="111"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="108"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="13" spans="2:31" ht="16">
       <c r="B13" s="91" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C13" s="14">
         <v>3</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="16" spans="2:31" ht="16">
       <c r="B16" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="14">
         <v>3</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="17" spans="2:31" ht="16">
       <c r="B17" s="90" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="14">
         <v>3</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="18" spans="2:31" ht="16">
       <c r="B18" s="90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="14">
         <v>3</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="19" spans="2:31" ht="16">
       <c r="B19" s="90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="14">
         <v>3</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="20" spans="2:31" ht="16">
       <c r="B20" s="90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="14">
         <v>3</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="21" spans="2:31" ht="16">
       <c r="B21" s="90" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="14">
         <v>3</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="22" spans="2:31" ht="16">
       <c r="B22" s="90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="14">
         <v>3</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="23" spans="2:31" ht="16">
       <c r="B23" s="90" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="14">
         <v>3</v>

</xml_diff>

<commit_message>
update grille de protection
</commit_message>
<xml_diff>
--- a/doc/grille-pointage.xlsx
+++ b/doc/grille-pointage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvanross/sources/log430/LOG430-STM/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC7E152-B332-FA40-8116-D4ABFB55A227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F7B190-8D3C-F045-9598-7BE4E00DAFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,9 +224,6 @@
     <t>Déduction total</t>
   </si>
   <si>
-    <t>S20223 - LOG430 Architecture logicielle</t>
-  </si>
-  <si>
     <t>Nombre total d'étudiant</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t xml:space="preserve"> OA2 - Promouvoir l'utilisation des données ouvertes</t>
+  </si>
+  <si>
+    <t>S20231 - LOG430 Architecture logicielle</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1392,8 @@
   </sheetPr>
   <dimension ref="B1:AG825"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1409,7 +1409,7 @@
   <sheetData>
     <row r="1" spans="2:31" ht="23.25" customHeight="1">
       <c r="B1" s="61" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1442,16 +1442,16 @@
         <v>33</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="89" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="11"/>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="3" spans="2:31" ht="23.25" customHeight="1">
       <c r="B3" s="96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="97">
         <v>1</v>
@@ -1717,7 +1717,7 @@
       <c r="D9" s="29"/>
       <c r="E9" s="51"/>
       <c r="F9" s="109" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="110"/>
       <c r="H9" s="110"/>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="10" spans="2:31" ht="27" customHeight="1" thickBot="1">
       <c r="B10" s="64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="106" t="s">
         <v>35</v>
@@ -1781,7 +1781,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>0</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="12" spans="2:31" ht="16">
       <c r="B12" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="38">
         <v>3</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="13" spans="2:31" ht="16">
       <c r="B13" s="91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="14">
         <v>3</v>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="14" spans="2:31" ht="16">
       <c r="B14" s="90" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="14">
         <v>3</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="15" spans="2:31" ht="16">
       <c r="B15" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="14">
         <v>3</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="16" spans="2:31" ht="16">
       <c r="B16" s="90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="14">
         <v>3</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="17" spans="2:31" ht="16">
       <c r="B17" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="14">
         <v>3</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="18" spans="2:31" ht="16">
       <c r="B18" s="90" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="14">
         <v>3</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="19" spans="2:31" ht="16">
       <c r="B19" s="90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="14">
         <v>3</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="20" spans="2:31" ht="16">
       <c r="B20" s="90" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="14">
         <v>3</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="21" spans="2:31" ht="16">
       <c r="B21" s="90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="14">
         <v>3</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="22" spans="2:31" ht="16">
       <c r="B22" s="90" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="14">
         <v>3</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="23" spans="2:31" ht="16">
       <c r="B23" s="90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="14">
         <v>3</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="51" spans="2:33" ht="17">
       <c r="B51" s="68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="99"/>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="61" spans="2:33" ht="17">
       <c r="B61" s="70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C61" s="30"/>
       <c r="D61" s="17"/>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="63" spans="2:33" ht="17">
       <c r="B63" s="69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" s="82">
         <f>+E61+H61+K61</f>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="64" spans="2:33" ht="17">
       <c r="B64" s="70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C64" s="53">
         <f>COUNTIF(B3:B8,"&lt;&gt;")</f>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="65" spans="2:33" ht="17">
       <c r="B65" s="69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C65" s="83">
         <f>+C63/C64</f>
@@ -4159,13 +4159,13 @@
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1">
       <c r="B66" s="75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C66" s="54">
         <v>33</v>
       </c>
       <c r="D66" s="84" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E66" s="85"/>
       <c r="F66" s="85"/>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="67" spans="2:33" ht="17">
       <c r="B67" s="75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C67" s="81">
         <f>+C65/C66*100</f>

</xml_diff>